<commit_message>
Updated version 02- Folder 01
</commit_message>
<xml_diff>
--- a/Database/Word Translations.xlsx
+++ b/Database/Word Translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SDGP_THE_Tyrants\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A27D40-DF5D-444F-BEDC-8D60713009C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8F7778-FB66-49BB-888E-C394169B1F24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1395" windowWidth="19485" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folder 01 Translations" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="707">
   <si>
     <t>Brahmi Word</t>
   </si>
@@ -2231,6 +2231,36 @@
   </si>
   <si>
     <t>One who owes his existence to Agni</t>
+  </si>
+  <si>
+    <t>Agiya</t>
+  </si>
+  <si>
+    <t>aghata</t>
+  </si>
+  <si>
+    <t>aca</t>
+  </si>
+  <si>
+    <t>bear</t>
+  </si>
+  <si>
+    <t>Aca-girika</t>
+  </si>
+  <si>
+    <t>bear-hill</t>
+  </si>
+  <si>
+    <t>Aca-nagaraka</t>
+  </si>
+  <si>
+    <t>Bear -Town</t>
+  </si>
+  <si>
+    <t>acariya</t>
+  </si>
+  <si>
+    <t>teacher</t>
   </si>
 </sst>
 </file>
@@ -2565,10 +2595,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2594,7 +2624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2605,7 +2635,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2619,7 +2649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -2630,7 +2660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2642,7 +2672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -2650,7 +2680,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -2661,7 +2691,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -2675,7 +2705,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2686,7 +2716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
@@ -2697,7 +2727,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
@@ -2708,7 +2738,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -2719,7 +2749,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -2730,7 +2760,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -2766,6 +2796,48 @@
       </c>
       <c r="B17" s="2" t="s">
         <v>696</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>706</v>
       </c>
     </row>
   </sheetData>
@@ -2871,7 +2943,7 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>46</v>
       </c>
@@ -2883,7 +2955,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>49</v>
       </c>
@@ -2895,7 +2967,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>52</v>
       </c>
@@ -2907,7 +2979,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>55</v>
       </c>
@@ -2919,7 +2991,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>58</v>
       </c>
@@ -2931,7 +3003,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>61</v>
       </c>
@@ -2943,7 +3015,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>64</v>
       </c>
@@ -2955,7 +3027,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>67</v>
       </c>
@@ -2965,7 +3037,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>69</v>
       </c>
@@ -2977,7 +3049,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>72</v>
       </c>
@@ -2989,7 +3061,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>75</v>
       </c>
@@ -3001,7 +3073,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>78</v>
       </c>
@@ -3013,7 +3085,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
Folder 01- 02nd page updated
</commit_message>
<xml_diff>
--- a/Database/Word Translations.xlsx
+++ b/Database/Word Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SDGP_THE_Tyrants\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F24109-9A77-4D40-8116-FCB7B6473138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB8F463-6F07-478B-9339-87B2BC5D5646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19725" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="877">
   <si>
     <t>Brahmi Word</t>
   </si>
@@ -2387,6 +2387,390 @@
   </si>
   <si>
     <t>a+ca+(ra+i)+ya</t>
+  </si>
+  <si>
+    <t>adiya</t>
+  </si>
+  <si>
+    <t>ananika</t>
+  </si>
+  <si>
+    <t>an irrigation expert</t>
+  </si>
+  <si>
+    <t>anikata</t>
+  </si>
+  <si>
+    <t>a body guard</t>
+  </si>
+  <si>
+    <t>ati</t>
+  </si>
+  <si>
+    <t>elephnat</t>
+  </si>
+  <si>
+    <t>ati-acariya</t>
+  </si>
+  <si>
+    <t>leader of a company of a elephnat trainers</t>
+  </si>
+  <si>
+    <t>ati-ajariya</t>
+  </si>
+  <si>
+    <t>trainer of elephants</t>
+  </si>
+  <si>
+    <t>ati-adika</t>
+  </si>
+  <si>
+    <t>superintendent of elephnats</t>
+  </si>
+  <si>
+    <t>Ati-matakaha</t>
+  </si>
+  <si>
+    <t>one whose mother is of the Atri or Atreya-gotra</t>
+  </si>
+  <si>
+    <t>atireka</t>
+  </si>
+  <si>
+    <t>remainder,residue</t>
+  </si>
+  <si>
+    <t>ativas'ika</t>
+  </si>
+  <si>
+    <t>pupil,disciple</t>
+  </si>
+  <si>
+    <t>atevas'ika</t>
+  </si>
+  <si>
+    <t>atevahika</t>
+  </si>
+  <si>
+    <t>adaka</t>
+  </si>
+  <si>
+    <t>Ada-kacaka</t>
+  </si>
+  <si>
+    <t>place name prefixed to a personal name</t>
+  </si>
+  <si>
+    <t>adakaha</t>
+  </si>
+  <si>
+    <t>adika</t>
+  </si>
+  <si>
+    <t>Adiliya</t>
+  </si>
+  <si>
+    <t>adeka</t>
+  </si>
+  <si>
+    <t>anagata</t>
+  </si>
+  <si>
+    <t>future</t>
+  </si>
+  <si>
+    <t>Anada</t>
+  </si>
+  <si>
+    <t>anu jete</t>
+  </si>
+  <si>
+    <t>Anudi</t>
+  </si>
+  <si>
+    <t>Anudi-gamasi</t>
+  </si>
+  <si>
+    <t>anubuti</t>
+  </si>
+  <si>
+    <t>Anurada</t>
+  </si>
+  <si>
+    <t>experience</t>
+  </si>
+  <si>
+    <t>growing,increasing</t>
+  </si>
+  <si>
+    <t>deputy of the alderman</t>
+  </si>
+  <si>
+    <t>a+(da+i)+ya</t>
+  </si>
+  <si>
+    <t>A+(na+u)+ra+da</t>
+  </si>
+  <si>
+    <t>a+(na+u)+(ba+u)+(ta+i)</t>
+  </si>
+  <si>
+    <t>A+(na+u)+(da+i)+ga+ma+(sa+i)</t>
+  </si>
+  <si>
+    <t>A+(na+u)+(da+i)</t>
+  </si>
+  <si>
+    <t>a+na+(na+i)+ka</t>
+  </si>
+  <si>
+    <t>a+(na+i)+ka+ta</t>
+  </si>
+  <si>
+    <t>a+(ta+i)</t>
+  </si>
+  <si>
+    <t>a+(na+u)+(ja+e)+(ta+e)</t>
+  </si>
+  <si>
+    <t>A+na+da</t>
+  </si>
+  <si>
+    <t>a+na+ga+ta</t>
+  </si>
+  <si>
+    <t>a+(da+e)+ka</t>
+  </si>
+  <si>
+    <t>A+(da+i)+(la+i)+ya</t>
+  </si>
+  <si>
+    <t>a+(da+i)+ka</t>
+  </si>
+  <si>
+    <t>a+da+ka+ha</t>
+  </si>
+  <si>
+    <t>A+da+ka+ca+ka</t>
+  </si>
+  <si>
+    <t>a+(ta+i)+a+ca+(ra+i)+ya</t>
+  </si>
+  <si>
+    <t>a+(ta+i)+a+ja+(ra+i)+ya</t>
+  </si>
+  <si>
+    <t>a+(ta+i)+a+(da+i)+ka</t>
+  </si>
+  <si>
+    <t>A+(ta+i)+ma+ta+ka+ha</t>
+  </si>
+  <si>
+    <t>a+(ta+i)+(ra+e)+ka</t>
+  </si>
+  <si>
+    <t>a+(ta+i)+va+(s'a+i)+ka</t>
+  </si>
+  <si>
+    <t>a+(ta+e)+va+(s'a+i)+ka</t>
+  </si>
+  <si>
+    <t>a+(ta+e)+va+(ha+i)+ka</t>
+  </si>
+  <si>
+    <t>a+da+ka</t>
+  </si>
+  <si>
+    <t>Anuradi</t>
+  </si>
+  <si>
+    <t>feminine of Anurada</t>
+  </si>
+  <si>
+    <t>Anuridi</t>
+  </si>
+  <si>
+    <t>Anula</t>
+  </si>
+  <si>
+    <t>name of a person</t>
+  </si>
+  <si>
+    <t>Anulapi</t>
+  </si>
+  <si>
+    <t>Anotata</t>
+  </si>
+  <si>
+    <t>name of a lake in the Himalayas</t>
+  </si>
+  <si>
+    <t>Anodi</t>
+  </si>
+  <si>
+    <t>faultless</t>
+  </si>
+  <si>
+    <t>Apaya</t>
+  </si>
+  <si>
+    <t>fearless</t>
+  </si>
+  <si>
+    <t>apara</t>
+  </si>
+  <si>
+    <t>another</t>
+  </si>
+  <si>
+    <t>aparimita</t>
+  </si>
+  <si>
+    <t>boundless</t>
+  </si>
+  <si>
+    <t>api</t>
+  </si>
+  <si>
+    <t>as a second member of ..</t>
+  </si>
+  <si>
+    <t>Aba</t>
+  </si>
+  <si>
+    <t>aba</t>
+  </si>
+  <si>
+    <t>Aba-adi</t>
+  </si>
+  <si>
+    <t>mango</t>
+  </si>
+  <si>
+    <t>mango tree channel</t>
+  </si>
+  <si>
+    <t>abaka</t>
+  </si>
+  <si>
+    <t>wife</t>
+  </si>
+  <si>
+    <t>Aba-tota</t>
+  </si>
+  <si>
+    <t>ferry named after a mango tree</t>
+  </si>
+  <si>
+    <t>Aba-nagara'na</t>
+  </si>
+  <si>
+    <t>residents or citizens or mebers of Aba-nagara</t>
+  </si>
+  <si>
+    <t>Aba-nagariyana</t>
+  </si>
+  <si>
+    <t>Abaya</t>
+  </si>
+  <si>
+    <t>Fearless</t>
+  </si>
+  <si>
+    <t>abala</t>
+  </si>
+  <si>
+    <t>sourness</t>
+  </si>
+  <si>
+    <t>Aba-velaka</t>
+  </si>
+  <si>
+    <t>Mango-tree-field</t>
+  </si>
+  <si>
+    <t>abi</t>
+  </si>
+  <si>
+    <t>an honoric title attached to names of princesses</t>
+  </si>
+  <si>
+    <t>Abijhatiya</t>
+  </si>
+  <si>
+    <t>high-born</t>
+  </si>
+  <si>
+    <t>A+(na+u)+ra+(da+i)</t>
+  </si>
+  <si>
+    <t>A+(ba+i)+jha+(ta+i)+ya</t>
+  </si>
+  <si>
+    <t>a+(ba+i)</t>
+  </si>
+  <si>
+    <t>A+ba+(va+e)+la+ka</t>
+  </si>
+  <si>
+    <t>a+ba+la</t>
+  </si>
+  <si>
+    <t>A+ba+ya</t>
+  </si>
+  <si>
+    <t>A+ba+na+ga+(ra+i)+ya+na</t>
+  </si>
+  <si>
+    <t>A+ba+na+ga+ra'+na</t>
+  </si>
+  <si>
+    <t>A+ba+(ta+o)+ta</t>
+  </si>
+  <si>
+    <t>a+ba+ka</t>
+  </si>
+  <si>
+    <t>A+ba+a+(da+i)</t>
+  </si>
+  <si>
+    <t>a+ba</t>
+  </si>
+  <si>
+    <t>A+ba</t>
+  </si>
+  <si>
+    <t>A+(na+u)+(ra+i)+(da+i)</t>
+  </si>
+  <si>
+    <t>A+(na+u)+la</t>
+  </si>
+  <si>
+    <t>A+(na+u)+la+(pa+i)</t>
+  </si>
+  <si>
+    <t>Anulaya</t>
+  </si>
+  <si>
+    <t>A+(na+u)+la+ya</t>
+  </si>
+  <si>
+    <t>A+(na+o)+ta+ta</t>
+  </si>
+  <si>
+    <t>A+(na+o)+(da+i)</t>
+  </si>
+  <si>
+    <t>A+pa+ya</t>
+  </si>
+  <si>
+    <t>a+pa+ra</t>
+  </si>
+  <si>
+    <t>a+pa+(ra+i)+(ma+i)+ta</t>
+  </si>
+  <si>
+    <t>a+(pa+i)</t>
   </si>
 </sst>
 </file>
@@ -2721,17 +3105,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
-    <col min="2" max="2" width="59" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="37.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
   </cols>
@@ -3127,6 +3511,498 @@
       </c>
       <c r="D37" t="s">
         <v>736</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="D38" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="B39" t="s">
+        <v>751</v>
+      </c>
+      <c r="D39" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="B40" t="s">
+        <v>753</v>
+      </c>
+      <c r="D40" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="B41" t="s">
+        <v>755</v>
+      </c>
+      <c r="D41" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="B42" t="s">
+        <v>757</v>
+      </c>
+      <c r="D42" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="B43" t="s">
+        <v>759</v>
+      </c>
+      <c r="D43" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="B44" t="s">
+        <v>761</v>
+      </c>
+      <c r="D44" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="B45" t="s">
+        <v>763</v>
+      </c>
+      <c r="D45" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="B46" t="s">
+        <v>765</v>
+      </c>
+      <c r="D46" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="B47" t="s">
+        <v>767</v>
+      </c>
+      <c r="D47" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="D48" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="D49" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="B50" t="s">
+        <v>728</v>
+      </c>
+      <c r="D50" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="B51" t="s">
+        <v>772</v>
+      </c>
+      <c r="D51" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="D52" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="D53" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="D54" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="D55" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="B56" t="s">
+        <v>778</v>
+      </c>
+      <c r="D56" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="D57" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="B58" t="s">
+        <v>787</v>
+      </c>
+      <c r="D58" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="B59" t="s">
+        <v>786</v>
+      </c>
+      <c r="D59" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="D60" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="B61" t="s">
+        <v>785</v>
+      </c>
+      <c r="D61" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="B62" t="s">
+        <v>571</v>
+      </c>
+      <c r="D62" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="B63" t="s">
+        <v>814</v>
+      </c>
+      <c r="D63" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="D64" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="B65" t="s">
+        <v>817</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="B66" t="s">
+        <v>437</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="B68" t="s">
+        <v>820</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="B69" t="s">
+        <v>822</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B70" t="s">
+        <v>824</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="B71" t="s">
+        <v>826</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="B72" t="s">
+        <v>828</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="B73" t="s">
+        <v>830</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="B74" t="s">
+        <v>824</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="B75" t="s">
+        <v>834</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="B76" t="s">
+        <v>835</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="B77" t="s">
+        <v>837</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="B78" t="s">
+        <v>839</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="B79" t="s">
+        <v>841</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="B81" t="s">
+        <v>844</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="B82" t="s">
+        <v>846</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="B83" t="s">
+        <v>848</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="B84" t="s">
+        <v>850</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="B85" t="s">
+        <v>852</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>854</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Folder 01 - Page 03 Updated
</commit_message>
<xml_diff>
--- a/Database/Word Translations.xlsx
+++ b/Database/Word Translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SDGP_THE_Tyrants\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB8F463-6F07-478B-9339-87B2BC5D5646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03AC7BC-A231-41A7-9136-563B6B54F5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19725" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10920" yWindow="765" windowWidth="8055" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folder 01 Translations" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,22 @@
     <sheet name="Folder 05 Translations" sheetId="5" r:id="rId5"/>
     <sheet name="Folder 06 Translations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="877">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="897">
   <si>
     <t>Brahmi Word</t>
   </si>
@@ -2771,6 +2781,66 @@
   </si>
   <si>
     <t>a+(pa+i)</t>
+  </si>
+  <si>
+    <t>S'onaya</t>
+  </si>
+  <si>
+    <t>S'onas'a</t>
+  </si>
+  <si>
+    <t>S'onaha</t>
+  </si>
+  <si>
+    <t>S'oniyagare</t>
+  </si>
+  <si>
+    <t>cave,empty house</t>
+  </si>
+  <si>
+    <t>S'onutara</t>
+  </si>
+  <si>
+    <t>combinataion of Sonu and Uttara</t>
+  </si>
+  <si>
+    <t>S'obanas'a</t>
+  </si>
+  <si>
+    <t>brilliant</t>
+  </si>
+  <si>
+    <t>S'obika</t>
+  </si>
+  <si>
+    <t>ornamental one</t>
+  </si>
+  <si>
+    <t>S'oma</t>
+  </si>
+  <si>
+    <t>moon</t>
+  </si>
+  <si>
+    <t>S'oma-dataha</t>
+  </si>
+  <si>
+    <t>given by Soma</t>
+  </si>
+  <si>
+    <t>S'oma-deva</t>
+  </si>
+  <si>
+    <t>one whose diety is Soma</t>
+  </si>
+  <si>
+    <t>S'omaliya</t>
+  </si>
+  <si>
+    <t>sagasa</t>
+  </si>
+  <si>
+    <t>Saga</t>
   </si>
 </sst>
 </file>
@@ -3105,10 +3175,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4003,6 +4073,92 @@
       </c>
       <c r="D85" s="2" t="s">
         <v>854</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="B89" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="B90" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="B91" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="B92" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="B93" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="B94" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>892</v>
+      </c>
+      <c r="B95" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Word Seperation - Folder 02
</commit_message>
<xml_diff>
--- a/Database/Word Translations.xlsx
+++ b/Database/Word Translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SDGP_THE_Tyrants\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6621EE4-0459-47EA-AA55-8CDCA703DD4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D4D644-E15E-4427-B9E2-55F1AA353131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folder 01 Translations" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="1188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="1263">
   <si>
     <t>Brahmi Word</t>
   </si>
@@ -3714,6 +3714,231 @@
   </si>
   <si>
     <t>Siva</t>
+  </si>
+  <si>
+    <t>Ka+na</t>
+  </si>
+  <si>
+    <t>Ka+na+ga+ma</t>
+  </si>
+  <si>
+    <t>Ka+na+(ga+u)+ta</t>
+  </si>
+  <si>
+    <t>Ka+na+(ta+i)+sa</t>
+  </si>
+  <si>
+    <t>Ka+na+da+ta</t>
+  </si>
+  <si>
+    <t>Ka+na+da+(sa+i)+ka</t>
+  </si>
+  <si>
+    <t>ka+na+(pa+e)+(da+i)+ka</t>
+  </si>
+  <si>
+    <t>Ka+na+ya</t>
+  </si>
+  <si>
+    <t>ka+na+ya+ta</t>
+  </si>
+  <si>
+    <t>Ka+na+sa</t>
+  </si>
+  <si>
+    <t>Ka+(na+i)+ka</t>
+  </si>
+  <si>
+    <t>[Ta+i]+sa</t>
+  </si>
+  <si>
+    <t>Ka+(na+i)+ka+na+(ta+i)+ya</t>
+  </si>
+  <si>
+    <t>ka+(na+i)+ya+ta</t>
+  </si>
+  <si>
+    <t>Ka+(na+i)+(ya+u)+ta+ga+ma</t>
+  </si>
+  <si>
+    <t>ka+(ta+i)+ka</t>
+  </si>
+  <si>
+    <t>Ka+(ta+i)+ya</t>
+  </si>
+  <si>
+    <t>Ka+da+(la+i)</t>
+  </si>
+  <si>
+    <t>Ka+(da+i)+(ta+i)+ha</t>
+  </si>
+  <si>
+    <t>Ka+pa+(la+i)</t>
+  </si>
+  <si>
+    <t>(Sa+i)+va</t>
+  </si>
+  <si>
+    <t>(sa+i)+dha+(ma+a)</t>
+  </si>
+  <si>
+    <t>(sa+i)+dha</t>
+  </si>
+  <si>
+    <t>(sa+i)+(da+a)+dha+(ma+m)</t>
+  </si>
+  <si>
+    <t>Ka+(pa+i)+la</t>
+  </si>
+  <si>
+    <t>Ka+ba+ra</t>
+  </si>
+  <si>
+    <t>Ka+(ba+o)+jha</t>
+  </si>
+  <si>
+    <t>Ka+(ba+o)+(jha+i)+ya</t>
+  </si>
+  <si>
+    <t>ka+ma</t>
+  </si>
+  <si>
+    <t>Ka+ma+(ca+u)+da+ha</t>
+  </si>
+  <si>
+    <t>ka+ma+ta</t>
+  </si>
+  <si>
+    <t>Ka+(ma+i)+na</t>
+  </si>
+  <si>
+    <t>ka+ya</t>
+  </si>
+  <si>
+    <t>ka+ra</t>
+  </si>
+  <si>
+    <t>Ka+ra+(ja+i)+(ha+i)+(na+i)+(Ta+i)+sa+ga+ma</t>
+  </si>
+  <si>
+    <t>Ka+ra+(ja+i)+(ha+i)+ka+ga+la</t>
+  </si>
+  <si>
+    <t>ka+ra+(pa+i)+ta</t>
+  </si>
+  <si>
+    <t>ka+ra+ha+ka</t>
+  </si>
+  <si>
+    <t>ka+(ra+i)+ta</t>
+  </si>
+  <si>
+    <t>ka+(ra+i)+ha, ka+(ra+i)+(ha+i)</t>
+  </si>
+  <si>
+    <t>Ka+la+(na+i)+ka</t>
+  </si>
+  <si>
+    <t>ka+la+(ha+i)</t>
+  </si>
+  <si>
+    <t>ka+(va+i)</t>
+  </si>
+  <si>
+    <t>Ka+sa+ka+sa</t>
+  </si>
+  <si>
+    <t>ka+sa+pa+(na+e)</t>
+  </si>
+  <si>
+    <t>Ka+sa+ba</t>
+  </si>
+  <si>
+    <t>Ka+sa+ba+na+ga+(ra+e)</t>
+  </si>
+  <si>
+    <t>Ka+sa+ba+sa</t>
+  </si>
+  <si>
+    <t>Ka+sa+ba+ha</t>
+  </si>
+  <si>
+    <t>Ka+sa+(ba+i)+ya</t>
+  </si>
+  <si>
+    <t>Ka+sa+(ba+e)</t>
+  </si>
+  <si>
+    <t>ka+ha+pa+(na+e)</t>
+  </si>
+  <si>
+    <t>Ka+ra+va+ha</t>
+  </si>
+  <si>
+    <t>ka+(ra+i)+(ta+e)</t>
+  </si>
+  <si>
+    <t>(Ka+i)+ta+ka+ya</t>
+  </si>
+  <si>
+    <t>(Ka+i)+ta+ha</t>
+  </si>
+  <si>
+    <t>(Ka+u)+jha</t>
+  </si>
+  <si>
+    <t>(Ka+u)+jha+ka</t>
+  </si>
+  <si>
+    <t>(ka+u)+ta</t>
+  </si>
+  <si>
+    <t>(Ka+u)+ta+ha+(ta+e)</t>
+  </si>
+  <si>
+    <t>(ka+u)+(ta+i)</t>
+  </si>
+  <si>
+    <t>(ka+u)+(ta+u)+(ba+i)+ka</t>
+  </si>
+  <si>
+    <t>(Ka+u)+da+ka</t>
+  </si>
+  <si>
+    <t>(Ka+u)+(na+i)+ka</t>
+  </si>
+  <si>
+    <t>(ka+u)+ta+ra+ga+ya</t>
+  </si>
+  <si>
+    <t>(Ka+u)+da+la</t>
+  </si>
+  <si>
+    <t>(ka+u)+ba+ka+ra</t>
+  </si>
+  <si>
+    <t>(Sa+i)+da+(va+i)+ya</t>
+  </si>
+  <si>
+    <t>(sa+i)+da+(ma+a)</t>
+  </si>
+  <si>
+    <t>(Ka+u)+ma+ra+(ta+i)+ha</t>
+  </si>
+  <si>
+    <t>(Ka+u)+ma+da+ta</t>
+  </si>
+  <si>
+    <t>(Ka+u)+(ba+i)+(la+i)+ya</t>
+  </si>
+  <si>
+    <t>(Ka+u)+(ba+i)+ra</t>
+  </si>
+  <si>
+    <t>(ka+u)+ba+la</t>
+  </si>
+  <si>
+    <t>(Ka+u)+ba+ra</t>
   </si>
 </sst>
 </file>
@@ -4083,8 +4308,8 @@
   </sheetPr>
   <dimension ref="A1:Z98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5101,14 +5326,15 @@
   </sheetPr>
   <dimension ref="A1:Z222"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5154,30 +5380,45 @@
       <c r="B2" s="17" t="s">
         <v>898</v>
       </c>
+      <c r="D2" s="17" t="s">
+        <v>1188</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>899</v>
       </c>
       <c r="B3" s="17"/>
+      <c r="D3" s="17" t="s">
+        <v>1189</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>900</v>
       </c>
       <c r="B4" s="17"/>
+      <c r="D4" s="17" t="s">
+        <v>1190</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>901</v>
       </c>
       <c r="B5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>1191</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>902</v>
       </c>
       <c r="B6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>1192</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
@@ -5186,6 +5427,9 @@
       <c r="B7" s="17" t="s">
         <v>904</v>
       </c>
+      <c r="D7" s="17" t="s">
+        <v>1193</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
@@ -5194,12 +5438,18 @@
       <c r="B8" s="17" t="s">
         <v>906</v>
       </c>
+      <c r="D8" s="17" t="s">
+        <v>1194</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>907</v>
       </c>
       <c r="B9" s="17"/>
+      <c r="D9" s="17" t="s">
+        <v>1195</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
@@ -5208,12 +5458,18 @@
       <c r="B10" s="17" t="s">
         <v>909</v>
       </c>
+      <c r="D10" s="17" t="s">
+        <v>1196</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>910</v>
       </c>
       <c r="B11" s="17"/>
+      <c r="D11" s="17" t="s">
+        <v>1197</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
@@ -5222,24 +5478,36 @@
       <c r="B12" s="17" t="s">
         <v>912</v>
       </c>
+      <c r="D12" s="17" t="s">
+        <v>1198</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>913</v>
       </c>
       <c r="B13" s="17"/>
+      <c r="D13" s="17" t="s">
+        <v>1199</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>914</v>
       </c>
       <c r="B14" s="17"/>
+      <c r="D14" s="17" t="s">
+        <v>1200</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>915</v>
       </c>
       <c r="B15" s="17"/>
+      <c r="D15" s="17" t="s">
+        <v>1201</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
@@ -5248,1392 +5516,2013 @@
       <c r="B16" s="17" t="s">
         <v>917</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="17" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>918</v>
       </c>
       <c r="B17" s="17"/>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="17" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>919</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="17" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>921</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>922</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="17" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>923</v>
       </c>
       <c r="B20" s="17"/>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="17" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>924</v>
       </c>
       <c r="B21" s="17"/>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="17" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>925</v>
       </c>
       <c r="B22" s="17"/>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="17" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>926</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>912</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="17" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>927</v>
       </c>
       <c r="B24" s="17"/>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="17" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>928</v>
       </c>
       <c r="B25" s="17"/>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="17" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>929</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="17" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>931</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="17" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>933</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="17" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>935</v>
       </c>
       <c r="B29" s="17"/>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="17" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>936</v>
       </c>
       <c r="B30" s="17"/>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="17" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>937</v>
       </c>
       <c r="B31" s="17"/>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="17" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>938</v>
       </c>
       <c r="B32" s="17"/>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="17" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>939</v>
       </c>
       <c r="B33" s="17"/>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="17" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>940</v>
       </c>
       <c r="B34" s="17"/>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="17" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>941</v>
       </c>
       <c r="B35" s="17" t="s">
         <v>942</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="17" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>943</v>
       </c>
       <c r="B36" s="17"/>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="17" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>944</v>
       </c>
       <c r="B37" s="17" t="s">
         <v>942</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="17" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>945</v>
       </c>
       <c r="B38" s="17"/>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="17" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>946</v>
       </c>
       <c r="B39" s="17"/>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="17" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>947</v>
       </c>
       <c r="B40" s="17"/>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="17" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>948</v>
       </c>
       <c r="B41" s="17"/>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="17" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>949</v>
       </c>
       <c r="B42" s="17"/>
-    </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="17" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>950</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>951</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="17" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>952</v>
       </c>
       <c r="B44" s="17"/>
-    </row>
-    <row r="45" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="17" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>953</v>
       </c>
       <c r="B45" s="17"/>
-    </row>
-    <row r="46" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="17" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>954</v>
       </c>
       <c r="B46" s="17"/>
-    </row>
-    <row r="47" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="17" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>955</v>
       </c>
       <c r="B47" s="17"/>
-    </row>
-    <row r="48" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="17" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>956</v>
       </c>
       <c r="B48" s="17"/>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="17" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>957</v>
       </c>
       <c r="B49" s="17"/>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="17" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>958</v>
       </c>
       <c r="B50" s="17" t="s">
         <v>959</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="17" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>960</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>959</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D51" s="17" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>961</v>
       </c>
       <c r="B52" s="17"/>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D52" s="17" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>962</v>
       </c>
       <c r="B53" s="17"/>
-    </row>
-    <row r="54" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D53" s="17" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>963</v>
       </c>
       <c r="B54" s="17" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D54" s="17" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>965</v>
       </c>
       <c r="B55" s="17" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="17" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>967</v>
       </c>
       <c r="B56" s="17" t="s">
         <v>968</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D56" s="17" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>969</v>
       </c>
       <c r="B57" s="17"/>
-    </row>
-    <row r="58" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="17" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>970</v>
       </c>
       <c r="B58" s="17"/>
-    </row>
-    <row r="59" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D58" s="17" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>971</v>
       </c>
       <c r="B59" s="17"/>
-    </row>
-    <row r="60" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D59" s="17" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>972</v>
       </c>
       <c r="B60" s="17"/>
-    </row>
-    <row r="61" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D60" s="17" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>973</v>
       </c>
       <c r="B61" s="17"/>
-    </row>
-    <row r="62" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D61" s="17" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
         <v>974</v>
       </c>
       <c r="B62" s="17" t="s">
         <v>975</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D62" s="17" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>976</v>
       </c>
       <c r="B63" s="17"/>
-    </row>
-    <row r="64" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="17" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
         <v>977</v>
       </c>
       <c r="B64" s="17"/>
-    </row>
-    <row r="65" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D64" s="17" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
         <v>978</v>
       </c>
       <c r="B65" s="17" t="s">
         <v>979</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D65" s="17" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
         <v>980</v>
       </c>
       <c r="B66" s="17" t="s">
         <v>912</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D66" s="17" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
         <v>981</v>
       </c>
       <c r="B67" s="17" t="s">
         <v>922</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D67" s="17" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>982</v>
       </c>
       <c r="B68" s="17"/>
-    </row>
-    <row r="69" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D68" s="17" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
         <v>983</v>
       </c>
       <c r="B69" s="17"/>
-    </row>
-    <row r="70" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D69" s="17" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
         <v>984</v>
       </c>
       <c r="B70" s="17"/>
-    </row>
-    <row r="71" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D70" s="17" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
         <v>985</v>
       </c>
       <c r="B71" s="17"/>
-    </row>
-    <row r="72" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D71" s="17" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>986</v>
       </c>
       <c r="B72" s="17"/>
-    </row>
-    <row r="73" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D72" s="17" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
         <v>987</v>
       </c>
       <c r="B73" s="17"/>
-    </row>
-    <row r="74" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D73" s="17" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
         <v>988</v>
       </c>
       <c r="B74" s="17" t="s">
         <v>989</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D74" s="17" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="17" t="s">
         <v>990</v>
       </c>
       <c r="B75" s="17"/>
-    </row>
-    <row r="76" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D75" s="17" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="17" t="s">
         <v>991</v>
       </c>
       <c r="B76" s="17" t="s">
         <v>992</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D76" s="17" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="17" t="s">
         <v>993</v>
       </c>
       <c r="B77" s="17" t="s">
         <v>992</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D77" s="17" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
         <v>994</v>
       </c>
       <c r="B78" s="17"/>
-    </row>
-    <row r="79" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D78" s="17" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="17" t="s">
         <v>995</v>
       </c>
       <c r="B79" s="17"/>
-    </row>
-    <row r="80" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D79" s="17" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
         <v>996</v>
       </c>
       <c r="B80" s="17" t="s">
         <v>997</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D80" s="17" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
         <v>998</v>
       </c>
       <c r="B81" s="17" t="s">
         <v>999</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D81" s="17" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
         <v>1000</v>
       </c>
       <c r="B82" s="17" t="s">
         <v>1001</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D82" s="17" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>1002</v>
       </c>
       <c r="B83" s="17" t="s">
         <v>1003</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="17" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
         <v>1004</v>
       </c>
       <c r="B84" s="17"/>
-    </row>
-    <row r="85" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D84" s="17" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
         <v>1005</v>
       </c>
       <c r="B85" s="17"/>
-    </row>
-    <row r="86" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D85" s="17" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
         <v>1006</v>
       </c>
       <c r="B86" s="17" t="s">
         <v>1007</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D86" s="17" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
         <v>1008</v>
       </c>
       <c r="B87" s="17"/>
-    </row>
-    <row r="88" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D87" s="17" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="17" t="s">
         <v>1009</v>
       </c>
       <c r="B88" s="17"/>
-    </row>
-    <row r="89" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D88" s="17" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
         <v>1010</v>
       </c>
       <c r="B89" s="17"/>
-    </row>
-    <row r="90" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D89" s="17" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
         <v>1011</v>
       </c>
       <c r="B90" s="17"/>
-    </row>
-    <row r="91" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D90" s="17" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
         <v>1012</v>
       </c>
       <c r="B91" s="17" t="s">
         <v>1013</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D91" s="17" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
         <v>1014</v>
       </c>
       <c r="B92" s="17" t="s">
         <v>1015</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D92" s="17" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>1016</v>
       </c>
       <c r="B93" s="17" t="s">
         <v>1017</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D93" s="17" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
         <v>1018</v>
       </c>
       <c r="B94" s="17"/>
-    </row>
-    <row r="95" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D94" s="17" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
         <v>1019</v>
       </c>
       <c r="B95" s="17" t="s">
         <v>1020</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D95" s="17" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="17" t="s">
         <v>1021</v>
       </c>
       <c r="B96" s="17"/>
-    </row>
-    <row r="97" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D96" s="17" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="17" t="s">
         <v>1022</v>
       </c>
       <c r="B97" s="17" t="s">
         <v>1023</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D97" s="17" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
         <v>1024</v>
       </c>
       <c r="B98" s="17"/>
-    </row>
-    <row r="99" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D98" s="17" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="17" t="s">
         <v>1025</v>
       </c>
       <c r="B99" s="17" t="s">
         <v>1026</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D99" s="17" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="17" t="s">
         <v>1027</v>
       </c>
       <c r="B100" s="17"/>
-    </row>
-    <row r="101" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D100" s="17" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="17" t="s">
         <v>1028</v>
       </c>
       <c r="B101" s="17" t="s">
         <v>1029</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D101" s="17" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="17" t="s">
         <v>1030</v>
       </c>
       <c r="B102" s="17"/>
-    </row>
-    <row r="103" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D102" s="17" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="17" t="s">
         <v>1031</v>
       </c>
       <c r="B103" s="17" t="s">
         <v>1032</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D103" s="17" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="17" t="s">
         <v>1033</v>
       </c>
       <c r="B104" s="17" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D104" s="17" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="17" t="s">
         <v>1035</v>
       </c>
       <c r="B105" s="17"/>
-    </row>
-    <row r="106" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D105" s="17" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="17" t="s">
         <v>1036</v>
       </c>
       <c r="B106" s="17"/>
-    </row>
-    <row r="107" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D106" s="17" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="17" t="s">
         <v>1037</v>
       </c>
       <c r="B107" s="17" t="s">
         <v>1038</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D107" s="17" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="17" t="s">
         <v>1039</v>
       </c>
       <c r="B108" s="17"/>
-    </row>
-    <row r="109" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D108" s="17" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="17" t="s">
         <v>1040</v>
       </c>
       <c r="B109" s="17"/>
-    </row>
-    <row r="110" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D109" s="17" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="17" t="s">
         <v>1041</v>
       </c>
       <c r="B110" s="17"/>
-    </row>
-    <row r="111" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D110" s="17" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" s="17" t="s">
         <v>1042</v>
       </c>
       <c r="B111" s="17" t="s">
         <v>1043</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D111" s="17" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="17" t="s">
         <v>1044</v>
       </c>
       <c r="B112" s="17"/>
-    </row>
-    <row r="113" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D112" s="17" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
         <v>1045</v>
       </c>
       <c r="B113" s="17"/>
-    </row>
-    <row r="114" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D113" s="17" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A114" s="17" t="s">
         <v>1046</v>
       </c>
       <c r="B114" s="17" t="s">
         <v>1047</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D114" s="17" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A115" s="17" t="s">
         <v>1048</v>
       </c>
       <c r="B115" s="17"/>
-    </row>
-    <row r="116" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D115" s="17" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A116" s="17" t="s">
         <v>1049</v>
       </c>
       <c r="B116" s="17"/>
-    </row>
-    <row r="117" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D116" s="17" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="17" t="s">
         <v>1050</v>
       </c>
       <c r="B117" s="17" t="s">
         <v>912</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D117" s="17" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="17" t="s">
         <v>1051</v>
       </c>
       <c r="B118" s="17"/>
-    </row>
-    <row r="119" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D118" s="17" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A119" s="17" t="s">
         <v>1052</v>
       </c>
       <c r="B119" s="17" t="s">
         <v>1053</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D119" s="17" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A120" s="17" t="s">
         <v>1054</v>
       </c>
       <c r="B120" s="17" t="s">
         <v>1055</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D120" s="17" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A121" s="17" t="s">
         <v>1056</v>
       </c>
       <c r="B121" s="17"/>
-    </row>
-    <row r="122" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D121" s="17" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A122" s="18" t="s">
         <v>1057</v>
       </c>
       <c r="B122" s="17"/>
-    </row>
-    <row r="123" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D122" s="18" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
         <v>1058</v>
       </c>
       <c r="B123" s="17"/>
-    </row>
-    <row r="124" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D123" s="17" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A124" s="17" t="s">
         <v>1059</v>
       </c>
       <c r="B124" s="17"/>
-    </row>
-    <row r="125" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D124" s="17" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A125" s="17" t="s">
         <v>1060</v>
       </c>
       <c r="B125" s="17"/>
-    </row>
-    <row r="126" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D125" s="17" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
         <v>1061</v>
       </c>
       <c r="B126" s="17" t="s">
         <v>1062</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D126" s="17" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A127" s="17" t="s">
         <v>1063</v>
       </c>
       <c r="B127" s="17" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D127" s="17" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="17" t="s">
         <v>1065</v>
       </c>
       <c r="B128" s="17"/>
-    </row>
-    <row r="129" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D128" s="17" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="17" t="s">
         <v>1066</v>
       </c>
       <c r="B129" s="17" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D129" s="17" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A130" s="17" t="s">
         <v>1067</v>
       </c>
       <c r="B130" s="17"/>
-    </row>
-    <row r="131" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D130" s="17" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A131" s="17" t="s">
         <v>1068</v>
       </c>
       <c r="B131" s="17" t="s">
         <v>1069</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D131" s="17" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A132" s="17" t="s">
         <v>1070</v>
       </c>
       <c r="B132" s="17" t="s">
         <v>1071</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D132" s="17" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="17" t="s">
         <v>1072</v>
       </c>
       <c r="B133" s="17"/>
-    </row>
-    <row r="134" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D133" s="17" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A134" s="17" t="s">
         <v>1073</v>
       </c>
       <c r="B134" s="17"/>
-    </row>
-    <row r="135" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D134" s="17" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A135" s="17" t="s">
         <v>1074</v>
       </c>
       <c r="B135" s="17"/>
-    </row>
-    <row r="136" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D135" s="17" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="17" t="s">
         <v>1075</v>
       </c>
       <c r="B136" s="17"/>
-    </row>
-    <row r="137" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D136" s="17" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A137" s="17" t="s">
         <v>1076</v>
       </c>
       <c r="B137" s="17" t="s">
         <v>1077</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D137" s="17" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A138" s="17" t="s">
         <v>1078</v>
       </c>
       <c r="B138" s="17" t="s">
         <v>1079</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D138" s="17" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A139" s="17" t="s">
         <v>1080</v>
       </c>
       <c r="B139" s="17"/>
-    </row>
-    <row r="140" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D139" s="17" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
         <v>1081</v>
       </c>
       <c r="B140" s="17"/>
-    </row>
-    <row r="141" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D140" s="17" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
         <v>1082</v>
       </c>
       <c r="B141" s="17" t="s">
         <v>1083</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D141" s="17" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="17" t="s">
         <v>1084</v>
       </c>
       <c r="B142" s="17"/>
-    </row>
-    <row r="143" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D142" s="17" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A143" s="17" t="s">
         <v>1085</v>
       </c>
       <c r="B143" s="17" t="s">
         <v>1086</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D143" s="17" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A144" s="17" t="s">
         <v>1087</v>
       </c>
       <c r="B144" s="17" t="s">
         <v>1088</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D144" s="17" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A145" s="17" t="s">
         <v>1089</v>
       </c>
       <c r="B145" s="17" t="s">
         <v>1090</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D145" s="17" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A146" s="17" t="s">
         <v>1091</v>
       </c>
       <c r="B146" s="17"/>
-    </row>
-    <row r="147" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D146" s="17" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
         <v>1092</v>
       </c>
       <c r="B147" s="17"/>
-    </row>
-    <row r="148" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D147" s="17" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A148" s="17" t="s">
         <v>1093</v>
       </c>
       <c r="B148" s="17"/>
-    </row>
-    <row r="149" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D148" s="17" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A149" s="17" t="s">
         <v>1094</v>
       </c>
       <c r="B149" s="17"/>
-    </row>
-    <row r="150" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D149" s="17" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A150" s="17" t="s">
         <v>1095</v>
       </c>
       <c r="B150" s="17"/>
-    </row>
-    <row r="151" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D150" s="17" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A151" s="17" t="s">
         <v>1096</v>
       </c>
       <c r="B151" s="17"/>
-    </row>
-    <row r="152" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D151" s="17" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A152" s="17" t="s">
         <v>1097</v>
       </c>
       <c r="B152" s="17"/>
-    </row>
-    <row r="153" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D152" s="17" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
         <v>1098</v>
       </c>
       <c r="B153" s="17" t="s">
         <v>1099</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D153" s="17" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
         <v>1100</v>
       </c>
       <c r="B154" s="17"/>
-    </row>
-    <row r="155" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D154" s="17" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A155" s="17" t="s">
         <v>1101</v>
       </c>
       <c r="B155" s="17"/>
-    </row>
-    <row r="156" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D155" s="17" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A156" s="17" t="s">
         <v>1102</v>
       </c>
       <c r="B156" s="17"/>
-    </row>
-    <row r="157" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D156" s="17" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A157" s="17" t="s">
         <v>1103</v>
       </c>
       <c r="B157" s="17"/>
-    </row>
-    <row r="158" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D157" s="17" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A158" s="17" t="s">
         <v>1104</v>
       </c>
       <c r="B158" s="17" t="s">
         <v>1105</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D158" s="17" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A159" s="17" t="s">
         <v>1106</v>
       </c>
       <c r="B159" s="17" t="s">
         <v>1107</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D159" s="17" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A160" s="17" t="s">
         <v>1108</v>
       </c>
       <c r="B160" s="17"/>
-    </row>
-    <row r="161" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D160" s="17" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A161" s="17" t="s">
         <v>1109</v>
       </c>
       <c r="B161" s="17"/>
-    </row>
-    <row r="162" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D161" s="17" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A162" s="17" t="s">
         <v>1110</v>
       </c>
       <c r="B162" s="17" t="s">
         <v>1105</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D162" s="17" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A163" s="17" t="s">
         <v>1111</v>
       </c>
       <c r="B163" s="17"/>
-    </row>
-    <row r="164" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D163" s="17" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A164" s="17" t="s">
         <v>1112</v>
       </c>
       <c r="B164" s="17"/>
-    </row>
-    <row r="165" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D164" s="17" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A165" s="17" t="s">
         <v>1113</v>
       </c>
       <c r="B165" s="17" t="s">
         <v>1114</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D165" s="17" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A166" s="17" t="s">
         <v>1115</v>
       </c>
       <c r="B166" s="17" t="s">
         <v>1116</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D166" s="17" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A167" s="17" t="s">
         <v>1117</v>
       </c>
       <c r="B167" s="17" t="s">
         <v>1118</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D167" s="17" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A168" s="17" t="s">
         <v>1119</v>
       </c>
       <c r="B168" s="17"/>
-    </row>
-    <row r="169" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D168" s="17" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A169" s="17" t="s">
         <v>1120</v>
       </c>
       <c r="B169" s="17"/>
-    </row>
-    <row r="170" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D169" s="17" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A170" s="17" t="s">
         <v>1121</v>
       </c>
       <c r="B170" s="17" t="s">
         <v>1122</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D170" s="17" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A171" s="17" t="s">
         <v>1123</v>
       </c>
       <c r="B171" s="17"/>
-    </row>
-    <row r="172" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D171" s="17" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A172" s="17" t="s">
         <v>1124</v>
       </c>
       <c r="B172" s="17" t="s">
         <v>1125</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D172" s="17" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A173" s="17" t="s">
         <v>1126</v>
       </c>
       <c r="B173" s="17"/>
-    </row>
-    <row r="174" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D173" s="17" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A174" s="17" t="s">
         <v>1127</v>
       </c>
       <c r="B174" s="17"/>
-    </row>
-    <row r="175" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D174" s="17" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A175" s="17" t="s">
         <v>1128</v>
       </c>
       <c r="B175" s="17"/>
-    </row>
-    <row r="176" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D175" s="17" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A176" s="17" t="s">
         <v>1129</v>
       </c>
       <c r="B176" s="17"/>
-    </row>
-    <row r="177" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D176" s="17" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A177" s="17" t="s">
         <v>1130</v>
       </c>
       <c r="B177" s="17"/>
-    </row>
-    <row r="178" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D177" s="17" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A178" s="17" t="s">
         <v>1131</v>
       </c>
       <c r="B178" s="17"/>
-    </row>
-    <row r="179" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D178" s="17" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A179" s="17" t="s">
         <v>1132</v>
       </c>
       <c r="B179" s="17"/>
-    </row>
-    <row r="180" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D179" s="17" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A180" s="17" t="s">
         <v>1133</v>
       </c>
       <c r="B180" s="17"/>
-    </row>
-    <row r="181" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D180" s="17" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A181" s="17" t="s">
         <v>1134</v>
       </c>
       <c r="B181" s="17"/>
-    </row>
-    <row r="182" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D181" s="17" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A182" s="17" t="s">
         <v>1135</v>
       </c>
       <c r="B182" s="17"/>
-    </row>
-    <row r="183" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D182" s="17" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A183" s="17" t="s">
         <v>1136</v>
       </c>
       <c r="B183" s="17"/>
-    </row>
-    <row r="184" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D183" s="17" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A184" s="17" t="s">
         <v>1137</v>
       </c>
       <c r="B184" s="17"/>
-    </row>
-    <row r="185" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D184" s="17" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A185" s="17" t="s">
         <v>1138</v>
       </c>
       <c r="B185" s="17"/>
-    </row>
-    <row r="186" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D185" s="17" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A186" s="17" t="s">
         <v>1139</v>
       </c>
       <c r="B186" s="17"/>
-    </row>
-    <row r="187" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D186" s="17" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A187" s="17" t="s">
         <v>1140</v>
       </c>
       <c r="B187" s="17"/>
-    </row>
-    <row r="188" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D187" s="17" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A188" s="17" t="s">
         <v>1141</v>
       </c>
       <c r="B188" s="17"/>
-    </row>
-    <row r="189" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D188" s="17" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A189" s="17" t="s">
         <v>1142</v>
       </c>
       <c r="B189" s="17" t="s">
         <v>1143</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D189" s="17" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A190" s="17" t="s">
         <v>1144</v>
       </c>
       <c r="B190" s="17"/>
-    </row>
-    <row r="191" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D190" s="17" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A191" s="17" t="s">
         <v>1145</v>
       </c>
       <c r="B191" s="17"/>
-    </row>
-    <row r="192" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D191" s="17" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A192" s="17" t="s">
         <v>1146</v>
       </c>
       <c r="B192" s="17"/>
-    </row>
-    <row r="193" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D192" s="17" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A193" s="17" t="s">
         <v>1147</v>
       </c>
       <c r="B193" s="17"/>
-    </row>
-    <row r="194" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D193" s="17" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A194" s="17" t="s">
         <v>1148</v>
       </c>
       <c r="B194" s="17"/>
-    </row>
-    <row r="195" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D194" s="17" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A195" s="17" t="s">
         <v>1149</v>
       </c>
       <c r="B195" s="17"/>
-    </row>
-    <row r="196" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D195" s="17" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A196" s="17" t="s">
         <v>1150</v>
       </c>
       <c r="B196" s="17"/>
-    </row>
-    <row r="197" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D196" s="17" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A197" s="17" t="s">
         <v>1151</v>
       </c>
       <c r="B197" s="17" t="s">
         <v>1152</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D197" s="17" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A198" s="17" t="s">
         <v>1153</v>
       </c>
       <c r="B198" s="17" t="s">
         <v>1154</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D198" s="17" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A199" s="17" t="s">
         <v>1155</v>
       </c>
       <c r="B199" s="17"/>
-    </row>
-    <row r="200" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D199" s="17" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A200" s="17" t="s">
         <v>1156</v>
       </c>
       <c r="B200" s="17"/>
-    </row>
-    <row r="201" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D200" s="17" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A201" s="17" t="s">
         <v>1157</v>
       </c>
       <c r="B201" s="17"/>
-    </row>
-    <row r="202" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D201" s="17" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A202" s="17" t="s">
         <v>1158</v>
       </c>
       <c r="B202" s="17" t="s">
         <v>1159</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D202" s="17" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A203" s="17" t="s">
         <v>1160</v>
       </c>
       <c r="B203" s="17"/>
-    </row>
-    <row r="204" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D203" s="17" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A204" s="17" t="s">
         <v>1161</v>
       </c>
       <c r="B204" s="17" t="s">
         <v>1162</v>
       </c>
-    </row>
-    <row r="205" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D204" s="17" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A205" s="17" t="s">
         <v>1163</v>
       </c>
       <c r="B205" s="17" t="s">
         <v>1164</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D205" s="17" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A206" s="17" t="s">
         <v>1165</v>
       </c>
       <c r="B206" s="17" t="s">
         <v>1166</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D206" s="17" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A207" s="17" t="s">
         <v>1167</v>
       </c>
       <c r="B207" s="17" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D207" s="17" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A208" s="17" t="s">
         <v>1168</v>
       </c>
       <c r="B208" s="17" t="s">
         <v>1169</v>
       </c>
-    </row>
-    <row r="209" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D208" s="17" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A209" s="17" t="s">
         <v>1170</v>
       </c>
       <c r="B209" s="17"/>
-    </row>
-    <row r="210" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D209" s="17" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A210" s="17" t="s">
         <v>1171</v>
       </c>
       <c r="B210" s="17"/>
-    </row>
-    <row r="211" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D210" s="17" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A211" s="17" t="s">
         <v>1172</v>
       </c>
       <c r="B211" s="17" t="s">
         <v>1173</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D211" s="17" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A212" s="17" t="s">
         <v>1174</v>
       </c>
       <c r="B212" s="17"/>
-    </row>
-    <row r="213" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D212" s="17" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A213" s="17" t="s">
         <v>1175</v>
       </c>
       <c r="B213" s="17" t="s">
         <v>1176</v>
       </c>
-    </row>
-    <row r="214" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D213" s="17" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A214" s="17" t="s">
         <v>1177</v>
       </c>
       <c r="B214" s="17" t="s">
         <v>1178</v>
       </c>
-    </row>
-    <row r="215" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D214" s="17" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A215" s="17" t="s">
         <v>1179</v>
       </c>
       <c r="B215" s="17" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="216" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D215" s="17" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A216" s="17" t="s">
         <v>1181</v>
       </c>
       <c r="B216" s="17"/>
-    </row>
-    <row r="217" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D216" s="17" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A217" s="17" t="s">
         <v>1182</v>
       </c>
       <c r="B217" s="17"/>
-    </row>
-    <row r="218" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D217" s="17" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A218" s="17" t="s">
         <v>1183</v>
       </c>
       <c r="B218" s="17" t="s">
         <v>1184</v>
       </c>
-    </row>
-    <row r="219" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D218" s="17" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A219" s="17" t="s">
         <v>1185</v>
       </c>
       <c r="B219" s="17"/>
-    </row>
-    <row r="220" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D219" s="17" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A220" s="17" t="s">
         <v>1186</v>
       </c>
       <c r="B220" s="17"/>
-    </row>
-    <row r="221" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D220" s="17" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A221" s="17" t="s">
         <v>1187</v>
       </c>
       <c r="B221" s="17"/>
-    </row>
-    <row r="222" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D221" s="17" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A222" s="17" t="s">
         <v>643</v>
       </c>
       <c r="B222" s="17"/>
+      <c r="D222" s="17" t="s">
+        <v>644</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Folder 02 - word seperation completed
</commit_message>
<xml_diff>
--- a/Database/Word Translations.xlsx
+++ b/Database/Word Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SDGP_THE_Tyrants\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D4D644-E15E-4427-B9E2-55F1AA353131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41289BD7-7A09-46EE-9A14-81E137C90025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="1263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="1406">
   <si>
     <t>Brahmi Word</t>
   </si>
@@ -3939,6 +3939,435 @@
   </si>
   <si>
     <t>(Ka+u)+ba+ra</t>
+  </si>
+  <si>
+    <t>(Ka+u)+ma+ra+da+ta+sa</t>
+  </si>
+  <si>
+    <t>(Ka+u)+ma+ra+sa</t>
+  </si>
+  <si>
+    <t>(Ka+u)+ma+ra+ha</t>
+  </si>
+  <si>
+    <t>(ka+u)+(ma+i)</t>
+  </si>
+  <si>
+    <t>(ka+u)+la</t>
+  </si>
+  <si>
+    <t>(ka+u)+(la+i)</t>
+  </si>
+  <si>
+    <t>(ka+u)+(la+i)+ka</t>
+  </si>
+  <si>
+    <t>(ka+e)+ta</t>
+  </si>
+  <si>
+    <t>(Ka+e)+ra+ha</t>
+  </si>
+  <si>
+    <t>(Ka+e)+la+(sa+e)</t>
+  </si>
+  <si>
+    <t>(Ka+o)+(ja+i)+ha+ra</t>
+  </si>
+  <si>
+    <t>(ka+o)+ta+ga+(ra+i)+ka</t>
+  </si>
+  <si>
+    <t>(ka+o)+ta+ya</t>
+  </si>
+  <si>
+    <t>(ka+o)+(ma+i)</t>
+  </si>
+  <si>
+    <t>(Ka+o)+la+ga+(ma+a)+(na+n)</t>
+  </si>
+  <si>
+    <t>(Ka+o)+(sa+i)+ka</t>
+  </si>
+  <si>
+    <t>(Ka+o)+(sa+i)+(ka+i)+ma+ta+ha</t>
+  </si>
+  <si>
+    <t>(ca+o)+(da+i)</t>
+  </si>
+  <si>
+    <t>(ca+o)+da+ka</t>
+  </si>
+  <si>
+    <t>(Ca+o)+(ra+i)+(ka+i)+ya</t>
+  </si>
+  <si>
+    <t>cha+(ta+u)</t>
+  </si>
+  <si>
+    <t>ja+na</t>
+  </si>
+  <si>
+    <t>(ja+i)+ta</t>
+  </si>
+  <si>
+    <t>(ja+e)+ta</t>
+  </si>
+  <si>
+    <t>Sa+ma+(na+i)+ya</t>
+  </si>
+  <si>
+    <t>sa+la</t>
+  </si>
+  <si>
+    <t>Sa+la</t>
+  </si>
+  <si>
+    <t>sa+va</t>
+  </si>
+  <si>
+    <t>Sa+va+(ta+o)+bha+(da+e)</t>
+  </si>
+  <si>
+    <t>sa+ha+tha+(ka+e)</t>
+  </si>
+  <si>
+    <t>(sa+i)</t>
+  </si>
+  <si>
+    <t>(sa+i)+ta</t>
+  </si>
+  <si>
+    <t>(sa+i)+da</t>
+  </si>
+  <si>
+    <t>(Ka+o)+(sa+i)+(ka+e)</t>
+  </si>
+  <si>
+    <t>kha+ra+(pa+i)+(ta+e)</t>
+  </si>
+  <si>
+    <t>Ga+ja+da+(ba+u)+ta+ka</t>
+  </si>
+  <si>
+    <t>ca+(da+a)+(la+a)</t>
+  </si>
+  <si>
+    <t>ca+ta</t>
+  </si>
+  <si>
+    <t>ca+ta+na</t>
+  </si>
+  <si>
+    <t>Ca+ta+ha</t>
+  </si>
+  <si>
+    <t>ca+tu</t>
+  </si>
+  <si>
+    <t>ca+da</t>
+  </si>
+  <si>
+    <t>Ca+da+ka</t>
+  </si>
+  <si>
+    <t>ca+da+ka</t>
+  </si>
+  <si>
+    <t>Ca+da+na+ha</t>
+  </si>
+  <si>
+    <t>ca+(da+u)</t>
+  </si>
+  <si>
+    <t>Ca+(da+e)</t>
+  </si>
+  <si>
+    <t>Ca+na+(ta+i)+sa+pa+va+ta</t>
+  </si>
+  <si>
+    <t>Ca+(na+i)+ga+(ma+i)ya</t>
+  </si>
+  <si>
+    <t>Ca+(na+i)+sa+ta</t>
+  </si>
+  <si>
+    <t>ca+ra</t>
+  </si>
+  <si>
+    <t>Ca+la+la</t>
+  </si>
+  <si>
+    <t>Ca+la+ha</t>
+  </si>
+  <si>
+    <t>Ca+(la+i)</t>
+  </si>
+  <si>
+    <t>Ca+(la+u)</t>
+  </si>
+  <si>
+    <t>Ca+ha+(na+i)+la+ya</t>
+  </si>
+  <si>
+    <t>(Ca+i)+ta</t>
+  </si>
+  <si>
+    <t>(ca+i)+ta+ka+ra</t>
+  </si>
+  <si>
+    <t>(Ca+i)+ta+ka+sa+na</t>
+  </si>
+  <si>
+    <t>(Ca+i)+ta+ka+ha</t>
+  </si>
+  <si>
+    <t>(Ca+i)+ta+(da+e)+(va+i)+ya</t>
+  </si>
+  <si>
+    <t>(Ca+i)+ta+(ga+u)+ta</t>
+  </si>
+  <si>
+    <t>(Ca+i)+ta+na+ga+ra+(ha+i)</t>
+  </si>
+  <si>
+    <t>(Ca+e)+(ra+e)+(ca+e)</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+a+(ya+i)+ma+ra+ha</t>
+  </si>
+  <si>
+    <t>(Ca+u)+(da+i)</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+(Ha+o)+na+ha</t>
+  </si>
+  <si>
+    <t>(Ca+u)+(da+i)+(Ta+i)+sa+ha</t>
+  </si>
+  <si>
+    <t>(Ca+u)+(da+i)+Na+ga+sa</t>
+  </si>
+  <si>
+    <t>(Ca+u)+(da+i)+ka</t>
+  </si>
+  <si>
+    <t>(Ca+u)+(da+u)+ta+ra</t>
+  </si>
+  <si>
+    <t>(Ca+u)+la</t>
+  </si>
+  <si>
+    <t>(Ca+u)+(la+u)</t>
+  </si>
+  <si>
+    <t>(Ca+u)+la+ta+ha</t>
+  </si>
+  <si>
+    <t>(ca+e)+(ta+i)+ya</t>
+  </si>
+  <si>
+    <t>(Ca+e)+ma</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+Ka+sa+ba+ha</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+(Ka+u)+ma+ra+ha</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+ga+(ma+i)+ka+ha</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+(Ta+i)+sa</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+Da+ta+ha</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+Na+ga+ha</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+(Ba+u)+da+ra+(ka+i)+ta</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+Ra+ka+sa</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+(Sa+i)+da+ha</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+(Sa+u)+da+sa+(na+e)</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+(Sa+u)+ma+na+ha</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+(Sa+o)+na+ha</t>
+  </si>
+  <si>
+    <t>(Ca+u)+da+Ha+(na+e)+ya+ha</t>
+  </si>
+  <si>
+    <t>ga+na</t>
+  </si>
+  <si>
+    <t>ga+na+ka</t>
+  </si>
+  <si>
+    <t>ga+na+ca+da+ka</t>
+  </si>
+  <si>
+    <t>ga+ta</t>
+  </si>
+  <si>
+    <t>Ga+da+ma+da+(na+e)</t>
+  </si>
+  <si>
+    <t>Ga+(da+i)+ya</t>
+  </si>
+  <si>
+    <t>ga+pa+ta+na</t>
+  </si>
+  <si>
+    <t>ga+pa+(ta+i)</t>
+  </si>
+  <si>
+    <t>ga+pa+(ta+u)+la</t>
+  </si>
+  <si>
+    <t>ga+(pa+i)+(ta+i)</t>
+  </si>
+  <si>
+    <t>ga+ma</t>
+  </si>
+  <si>
+    <t>ga+ma+ka</t>
+  </si>
+  <si>
+    <t>Ga+ma+(na+i)</t>
+  </si>
+  <si>
+    <t>ga+ma+(na+i)</t>
+  </si>
+  <si>
+    <t>ga+ma+(sa+i)</t>
+  </si>
+  <si>
+    <t>ga+ma+(ha+i)</t>
+  </si>
+  <si>
+    <t>ga+(ma+i)+ka</t>
+  </si>
+  <si>
+    <t>ga+(ma+i)+ya</t>
+  </si>
+  <si>
+    <t>Ga+ra+(da+i)+da+ga+ma</t>
+  </si>
+  <si>
+    <t>ga+la</t>
+  </si>
+  <si>
+    <t>ga+ha+pa+(ta+i)</t>
+  </si>
+  <si>
+    <t>ga+ha+pa+(ta+i)+na+ka</t>
+  </si>
+  <si>
+    <t>ga+(ha+e)</t>
+  </si>
+  <si>
+    <t>(ga+i)+(ra+i)</t>
+  </si>
+  <si>
+    <t>(Ga+i)+(ra+i)+(ta+i)+sa+ga+ma</t>
+  </si>
+  <si>
+    <t>(Ga+i)+(ra+i)+va+(ja+e)</t>
+  </si>
+  <si>
+    <t>(Ga+i)+(la+i)+ka</t>
+  </si>
+  <si>
+    <t>(Ga+u)+ta+ka</t>
+  </si>
+  <si>
+    <t>(Ga+u)+da+ha</t>
+  </si>
+  <si>
+    <t>(Ga+u)+ta</t>
+  </si>
+  <si>
+    <t>(Ga+u)+ta+ya</t>
+  </si>
+  <si>
+    <t>(Ga+u)+ta+sa</t>
+  </si>
+  <si>
+    <t>(Ga+u)+ta+ha</t>
+  </si>
+  <si>
+    <t>gha+(ma+i)+ka</t>
+  </si>
+  <si>
+    <t>(ga+o)+ha</t>
+  </si>
+  <si>
+    <t>(ga+o)+va+ka</t>
+  </si>
+  <si>
+    <t>(Ga+o)+(ba+u)+(ta+i)+ya</t>
+  </si>
+  <si>
+    <t>(Ga+o)+pa+la+ha</t>
+  </si>
+  <si>
+    <t>(Ga+o)+pa+ha</t>
+  </si>
+  <si>
+    <t>(ga+o)+pa+ka</t>
+  </si>
+  <si>
+    <t>(Ga+o)+da+ta</t>
+  </si>
+  <si>
+    <t>(Ga+o)+(ta+i)+ma+ta+ha</t>
+  </si>
+  <si>
+    <t>(Ga+o)+ta+ma</t>
+  </si>
+  <si>
+    <t>(Ga+o)+da+ha</t>
+  </si>
+  <si>
+    <t>(ga+o)+da</t>
+  </si>
+  <si>
+    <t>(ga+o)+ta</t>
+  </si>
+  <si>
+    <t>(ga+u)+(ta+i)+ya</t>
+  </si>
+  <si>
+    <t>(Ga+u)+(ta+e)+na</t>
+  </si>
+  <si>
+    <t>(Ga+u)+ra+ya</t>
+  </si>
+  <si>
+    <t>(Ga+u)+ra+ha</t>
+  </si>
+  <si>
+    <t>(ga+u)+(sa+e)</t>
+  </si>
+  <si>
+    <t>(ga+u)+ha</t>
+  </si>
+  <si>
+    <t>(Ga+o)+ka+na+ga+ma+ka+va+(va+i)</t>
   </si>
 </sst>
 </file>
@@ -5326,8 +5755,8 @@
   </sheetPr>
   <dimension ref="A1:Z222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
+      <selection activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6048,7 +6477,7 @@
       </c>
       <c r="B71" s="17"/>
       <c r="D71" s="17" t="s">
-        <v>985</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6057,7 +6486,7 @@
       </c>
       <c r="B72" s="17"/>
       <c r="D72" s="17" t="s">
-        <v>986</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6066,7 +6495,7 @@
       </c>
       <c r="B73" s="17"/>
       <c r="D73" s="17" t="s">
-        <v>987</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6077,7 +6506,7 @@
         <v>989</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>988</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6086,7 +6515,7 @@
       </c>
       <c r="B75" s="17"/>
       <c r="D75" s="17" t="s">
-        <v>990</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6097,7 +6526,7 @@
         <v>992</v>
       </c>
       <c r="D76" s="17" t="s">
-        <v>991</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6108,7 +6537,7 @@
         <v>992</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>993</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6117,7 +6546,7 @@
       </c>
       <c r="B78" s="17"/>
       <c r="D78" s="17" t="s">
-        <v>994</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6126,7 +6555,7 @@
       </c>
       <c r="B79" s="17"/>
       <c r="D79" s="17" t="s">
-        <v>995</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6137,7 +6566,7 @@
         <v>997</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>996</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6148,7 +6577,7 @@
         <v>999</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>998</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6159,7 +6588,7 @@
         <v>1001</v>
       </c>
       <c r="D82" s="17" t="s">
-        <v>1000</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6170,7 +6599,7 @@
         <v>1003</v>
       </c>
       <c r="D83" s="17" t="s">
-        <v>1002</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6179,7 +6608,7 @@
       </c>
       <c r="B84" s="17"/>
       <c r="D84" s="17" t="s">
-        <v>1004</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6188,7 +6617,7 @@
       </c>
       <c r="B85" s="17"/>
       <c r="D85" s="17" t="s">
-        <v>1005</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6199,7 +6628,7 @@
         <v>1007</v>
       </c>
       <c r="D86" s="17" t="s">
-        <v>1006</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6208,7 +6637,7 @@
       </c>
       <c r="B87" s="17"/>
       <c r="D87" s="17" t="s">
-        <v>1008</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6217,7 +6646,7 @@
       </c>
       <c r="B88" s="17"/>
       <c r="D88" s="17" t="s">
-        <v>1009</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6226,7 +6655,7 @@
       </c>
       <c r="B89" s="17"/>
       <c r="D89" s="17" t="s">
-        <v>1010</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6235,7 +6664,7 @@
       </c>
       <c r="B90" s="17"/>
       <c r="D90" s="17" t="s">
-        <v>1011</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6246,7 +6675,7 @@
         <v>1013</v>
       </c>
       <c r="D91" s="17" t="s">
-        <v>1012</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6257,7 +6686,7 @@
         <v>1015</v>
       </c>
       <c r="D92" s="17" t="s">
-        <v>1014</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6268,7 +6697,7 @@
         <v>1017</v>
       </c>
       <c r="D93" s="17" t="s">
-        <v>1016</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6277,7 +6706,7 @@
       </c>
       <c r="B94" s="17"/>
       <c r="D94" s="17" t="s">
-        <v>1018</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6288,7 +6717,7 @@
         <v>1020</v>
       </c>
       <c r="D95" s="17" t="s">
-        <v>1019</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6297,7 +6726,7 @@
       </c>
       <c r="B96" s="17"/>
       <c r="D96" s="17" t="s">
-        <v>1021</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6308,7 +6737,7 @@
         <v>1023</v>
       </c>
       <c r="D97" s="17" t="s">
-        <v>1022</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6317,7 +6746,7 @@
       </c>
       <c r="B98" s="17"/>
       <c r="D98" s="17" t="s">
-        <v>1024</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6328,7 +6757,7 @@
         <v>1026</v>
       </c>
       <c r="D99" s="17" t="s">
-        <v>1025</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6337,7 +6766,7 @@
       </c>
       <c r="B100" s="17"/>
       <c r="D100" s="17" t="s">
-        <v>1027</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6348,7 +6777,7 @@
         <v>1029</v>
       </c>
       <c r="D101" s="17" t="s">
-        <v>1028</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6357,7 +6786,7 @@
       </c>
       <c r="B102" s="17"/>
       <c r="D102" s="17" t="s">
-        <v>1030</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6368,7 +6797,7 @@
         <v>1032</v>
       </c>
       <c r="D103" s="17" t="s">
-        <v>1031</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6379,7 +6808,7 @@
         <v>1034</v>
       </c>
       <c r="D104" s="17" t="s">
-        <v>1033</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6388,7 +6817,7 @@
       </c>
       <c r="B105" s="17"/>
       <c r="D105" s="17" t="s">
-        <v>1035</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6397,7 +6826,7 @@
       </c>
       <c r="B106" s="17"/>
       <c r="D106" s="17" t="s">
-        <v>1036</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6408,7 +6837,7 @@
         <v>1038</v>
       </c>
       <c r="D107" s="17" t="s">
-        <v>1037</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6417,7 +6846,7 @@
       </c>
       <c r="B108" s="17"/>
       <c r="D108" s="17" t="s">
-        <v>1039</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6426,7 +6855,7 @@
       </c>
       <c r="B109" s="17"/>
       <c r="D109" s="17" t="s">
-        <v>1040</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6435,7 +6864,7 @@
       </c>
       <c r="B110" s="17"/>
       <c r="D110" s="17" t="s">
-        <v>1041</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6446,7 +6875,7 @@
         <v>1043</v>
       </c>
       <c r="D111" s="17" t="s">
-        <v>1042</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6455,7 +6884,7 @@
       </c>
       <c r="B112" s="17"/>
       <c r="D112" s="17" t="s">
-        <v>1044</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6464,7 +6893,7 @@
       </c>
       <c r="B113" s="17"/>
       <c r="D113" s="17" t="s">
-        <v>1045</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6475,7 +6904,7 @@
         <v>1047</v>
       </c>
       <c r="D114" s="17" t="s">
-        <v>1046</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6484,7 +6913,7 @@
       </c>
       <c r="B115" s="17"/>
       <c r="D115" s="17" t="s">
-        <v>1048</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6493,7 +6922,7 @@
       </c>
       <c r="B116" s="17"/>
       <c r="D116" s="17" t="s">
-        <v>1049</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6504,7 +6933,7 @@
         <v>912</v>
       </c>
       <c r="D117" s="17" t="s">
-        <v>1050</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6513,7 +6942,7 @@
       </c>
       <c r="B118" s="17"/>
       <c r="D118" s="17" t="s">
-        <v>1051</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6524,7 +6953,7 @@
         <v>1053</v>
       </c>
       <c r="D119" s="17" t="s">
-        <v>1052</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6535,7 +6964,7 @@
         <v>1055</v>
       </c>
       <c r="D120" s="17" t="s">
-        <v>1054</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6544,7 +6973,7 @@
       </c>
       <c r="B121" s="17"/>
       <c r="D121" s="17" t="s">
-        <v>1056</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6553,7 +6982,7 @@
       </c>
       <c r="B122" s="17"/>
       <c r="D122" s="18" t="s">
-        <v>1057</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6562,7 +6991,7 @@
       </c>
       <c r="B123" s="17"/>
       <c r="D123" s="17" t="s">
-        <v>1058</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6571,7 +7000,7 @@
       </c>
       <c r="B124" s="17"/>
       <c r="D124" s="17" t="s">
-        <v>1059</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6580,7 +7009,7 @@
       </c>
       <c r="B125" s="17"/>
       <c r="D125" s="17" t="s">
-        <v>1060</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6591,7 +7020,7 @@
         <v>1062</v>
       </c>
       <c r="D126" s="17" t="s">
-        <v>1061</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6602,7 +7031,7 @@
         <v>1064</v>
       </c>
       <c r="D127" s="17" t="s">
-        <v>1063</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6611,7 +7040,7 @@
       </c>
       <c r="B128" s="17"/>
       <c r="D128" s="17" t="s">
-        <v>1065</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6622,7 +7051,7 @@
         <v>594</v>
       </c>
       <c r="D129" s="17" t="s">
-        <v>1066</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6631,7 +7060,7 @@
       </c>
       <c r="B130" s="17"/>
       <c r="D130" s="17" t="s">
-        <v>1067</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6642,7 +7071,7 @@
         <v>1069</v>
       </c>
       <c r="D131" s="17" t="s">
-        <v>1068</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6653,7 +7082,7 @@
         <v>1071</v>
       </c>
       <c r="D132" s="17" t="s">
-        <v>1070</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6662,7 +7091,7 @@
       </c>
       <c r="B133" s="17"/>
       <c r="D133" s="17" t="s">
-        <v>1072</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6671,7 +7100,7 @@
       </c>
       <c r="B134" s="17"/>
       <c r="D134" s="17" t="s">
-        <v>1073</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6680,7 +7109,7 @@
       </c>
       <c r="B135" s="17"/>
       <c r="D135" s="17" t="s">
-        <v>1074</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6689,7 +7118,7 @@
       </c>
       <c r="B136" s="17"/>
       <c r="D136" s="17" t="s">
-        <v>1075</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6700,7 +7129,7 @@
         <v>1077</v>
       </c>
       <c r="D137" s="17" t="s">
-        <v>1076</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6711,7 +7140,7 @@
         <v>1079</v>
       </c>
       <c r="D138" s="17" t="s">
-        <v>1078</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6720,7 +7149,7 @@
       </c>
       <c r="B139" s="17"/>
       <c r="D139" s="17" t="s">
-        <v>1080</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6729,7 +7158,7 @@
       </c>
       <c r="B140" s="17"/>
       <c r="D140" s="17" t="s">
-        <v>1081</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6740,7 +7169,7 @@
         <v>1083</v>
       </c>
       <c r="D141" s="17" t="s">
-        <v>1082</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6749,7 +7178,7 @@
       </c>
       <c r="B142" s="17"/>
       <c r="D142" s="17" t="s">
-        <v>1084</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6760,7 +7189,7 @@
         <v>1086</v>
       </c>
       <c r="D143" s="17" t="s">
-        <v>1085</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6782,7 +7211,7 @@
         <v>1090</v>
       </c>
       <c r="D145" s="17" t="s">
-        <v>1089</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6791,7 +7220,7 @@
       </c>
       <c r="B146" s="17"/>
       <c r="D146" s="17" t="s">
-        <v>1091</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6800,7 +7229,7 @@
       </c>
       <c r="B147" s="17"/>
       <c r="D147" s="17" t="s">
-        <v>1092</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6809,7 +7238,7 @@
       </c>
       <c r="B148" s="17"/>
       <c r="D148" s="17" t="s">
-        <v>1093</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6818,7 +7247,7 @@
       </c>
       <c r="B149" s="17"/>
       <c r="D149" s="17" t="s">
-        <v>1094</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6827,7 +7256,7 @@
       </c>
       <c r="B150" s="17"/>
       <c r="D150" s="17" t="s">
-        <v>1095</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6836,7 +7265,7 @@
       </c>
       <c r="B151" s="17"/>
       <c r="D151" s="17" t="s">
-        <v>1096</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6845,7 +7274,7 @@
       </c>
       <c r="B152" s="17"/>
       <c r="D152" s="17" t="s">
-        <v>1097</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6856,7 +7285,7 @@
         <v>1099</v>
       </c>
       <c r="D153" s="17" t="s">
-        <v>1098</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6865,7 +7294,7 @@
       </c>
       <c r="B154" s="17"/>
       <c r="D154" s="17" t="s">
-        <v>1100</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6874,7 +7303,7 @@
       </c>
       <c r="B155" s="17"/>
       <c r="D155" s="17" t="s">
-        <v>1101</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6883,7 +7312,7 @@
       </c>
       <c r="B156" s="17"/>
       <c r="D156" s="17" t="s">
-        <v>1102</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6892,7 +7321,7 @@
       </c>
       <c r="B157" s="17"/>
       <c r="D157" s="17" t="s">
-        <v>1103</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6903,7 +7332,7 @@
         <v>1105</v>
       </c>
       <c r="D158" s="17" t="s">
-        <v>1104</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6914,7 +7343,7 @@
         <v>1107</v>
       </c>
       <c r="D159" s="17" t="s">
-        <v>1106</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6923,7 +7352,7 @@
       </c>
       <c r="B160" s="17"/>
       <c r="D160" s="17" t="s">
-        <v>1108</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6932,7 +7361,7 @@
       </c>
       <c r="B161" s="17"/>
       <c r="D161" s="17" t="s">
-        <v>1109</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6943,7 +7372,7 @@
         <v>1105</v>
       </c>
       <c r="D162" s="17" t="s">
-        <v>1110</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6952,7 +7381,7 @@
       </c>
       <c r="B163" s="17"/>
       <c r="D163" s="17" t="s">
-        <v>1111</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6961,7 +7390,7 @@
       </c>
       <c r="B164" s="17"/>
       <c r="D164" s="17" t="s">
-        <v>1112</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6972,7 +7401,7 @@
         <v>1114</v>
       </c>
       <c r="D165" s="17" t="s">
-        <v>1113</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6983,7 +7412,7 @@
         <v>1116</v>
       </c>
       <c r="D166" s="17" t="s">
-        <v>1115</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6994,7 +7423,7 @@
         <v>1118</v>
       </c>
       <c r="D167" s="17" t="s">
-        <v>1117</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7003,7 +7432,7 @@
       </c>
       <c r="B168" s="17"/>
       <c r="D168" s="17" t="s">
-        <v>1119</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7012,7 +7441,7 @@
       </c>
       <c r="B169" s="17"/>
       <c r="D169" s="17" t="s">
-        <v>1120</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7023,7 +7452,7 @@
         <v>1122</v>
       </c>
       <c r="D170" s="17" t="s">
-        <v>1121</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7032,7 +7461,7 @@
       </c>
       <c r="B171" s="17"/>
       <c r="D171" s="17" t="s">
-        <v>1123</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7043,7 +7472,7 @@
         <v>1125</v>
       </c>
       <c r="D172" s="17" t="s">
-        <v>1124</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7052,7 +7481,7 @@
       </c>
       <c r="B173" s="17"/>
       <c r="D173" s="17" t="s">
-        <v>1126</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7061,7 +7490,7 @@
       </c>
       <c r="B174" s="17"/>
       <c r="D174" s="17" t="s">
-        <v>1127</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7070,7 +7499,7 @@
       </c>
       <c r="B175" s="17"/>
       <c r="D175" s="17" t="s">
-        <v>1128</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7079,7 +7508,7 @@
       </c>
       <c r="B176" s="17"/>
       <c r="D176" s="17" t="s">
-        <v>1129</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7088,7 +7517,7 @@
       </c>
       <c r="B177" s="17"/>
       <c r="D177" s="17" t="s">
-        <v>1130</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7097,7 +7526,7 @@
       </c>
       <c r="B178" s="17"/>
       <c r="D178" s="17" t="s">
-        <v>1131</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7106,7 +7535,7 @@
       </c>
       <c r="B179" s="17"/>
       <c r="D179" s="17" t="s">
-        <v>1132</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7115,7 +7544,7 @@
       </c>
       <c r="B180" s="17"/>
       <c r="D180" s="17" t="s">
-        <v>1133</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7124,7 +7553,7 @@
       </c>
       <c r="B181" s="17"/>
       <c r="D181" s="17" t="s">
-        <v>1134</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7133,7 +7562,7 @@
       </c>
       <c r="B182" s="17"/>
       <c r="D182" s="17" t="s">
-        <v>1135</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7142,7 +7571,7 @@
       </c>
       <c r="B183" s="17"/>
       <c r="D183" s="17" t="s">
-        <v>1136</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7151,7 +7580,7 @@
       </c>
       <c r="B184" s="17"/>
       <c r="D184" s="17" t="s">
-        <v>1137</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7160,7 +7589,7 @@
       </c>
       <c r="B185" s="17"/>
       <c r="D185" s="17" t="s">
-        <v>1138</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7169,7 +7598,7 @@
       </c>
       <c r="B186" s="17"/>
       <c r="D186" s="17" t="s">
-        <v>1139</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7178,7 +7607,7 @@
       </c>
       <c r="B187" s="17"/>
       <c r="D187" s="17" t="s">
-        <v>1140</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7187,7 +7616,7 @@
       </c>
       <c r="B188" s="17"/>
       <c r="D188" s="17" t="s">
-        <v>1141</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7198,7 +7627,7 @@
         <v>1143</v>
       </c>
       <c r="D189" s="17" t="s">
-        <v>1142</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7207,7 +7636,7 @@
       </c>
       <c r="B190" s="17"/>
       <c r="D190" s="17" t="s">
-        <v>1144</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7216,7 +7645,7 @@
       </c>
       <c r="B191" s="17"/>
       <c r="D191" s="17" t="s">
-        <v>1145</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7225,7 +7654,7 @@
       </c>
       <c r="B192" s="17"/>
       <c r="D192" s="17" t="s">
-        <v>1146</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7234,7 +7663,7 @@
       </c>
       <c r="B193" s="17"/>
       <c r="D193" s="17" t="s">
-        <v>1147</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7243,7 +7672,7 @@
       </c>
       <c r="B194" s="17"/>
       <c r="D194" s="17" t="s">
-        <v>1148</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7252,7 +7681,7 @@
       </c>
       <c r="B195" s="17"/>
       <c r="D195" s="17" t="s">
-        <v>1149</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7261,7 +7690,7 @@
       </c>
       <c r="B196" s="17"/>
       <c r="D196" s="17" t="s">
-        <v>1150</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7272,7 +7701,7 @@
         <v>1152</v>
       </c>
       <c r="D197" s="17" t="s">
-        <v>1151</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7283,7 +7712,7 @@
         <v>1154</v>
       </c>
       <c r="D198" s="17" t="s">
-        <v>1153</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7301,7 +7730,7 @@
       </c>
       <c r="B200" s="17"/>
       <c r="D200" s="17" t="s">
-        <v>1156</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7310,7 +7739,7 @@
       </c>
       <c r="B201" s="17"/>
       <c r="D201" s="17" t="s">
-        <v>1157</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7321,7 +7750,7 @@
         <v>1159</v>
       </c>
       <c r="D202" s="17" t="s">
-        <v>1158</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7330,7 +7759,7 @@
       </c>
       <c r="B203" s="17"/>
       <c r="D203" s="17" t="s">
-        <v>1160</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7341,7 +7770,7 @@
         <v>1162</v>
       </c>
       <c r="D204" s="17" t="s">
-        <v>1161</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7352,7 +7781,7 @@
         <v>1164</v>
       </c>
       <c r="D205" s="17" t="s">
-        <v>1163</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7363,7 +7792,7 @@
         <v>1166</v>
       </c>
       <c r="D206" s="17" t="s">
-        <v>1165</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7374,7 +7803,7 @@
         <v>112</v>
       </c>
       <c r="D207" s="17" t="s">
-        <v>1167</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7385,7 +7814,7 @@
         <v>1169</v>
       </c>
       <c r="D208" s="17" t="s">
-        <v>1168</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7394,7 +7823,7 @@
       </c>
       <c r="B209" s="17"/>
       <c r="D209" s="17" t="s">
-        <v>1170</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7403,7 +7832,7 @@
       </c>
       <c r="B210" s="17"/>
       <c r="D210" s="17" t="s">
-        <v>1171</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7414,7 +7843,7 @@
         <v>1173</v>
       </c>
       <c r="D211" s="17" t="s">
-        <v>1172</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7423,7 +7852,7 @@
       </c>
       <c r="B212" s="17"/>
       <c r="D212" s="17" t="s">
-        <v>1174</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7434,7 +7863,7 @@
         <v>1176</v>
       </c>
       <c r="D213" s="17" t="s">
-        <v>1175</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7445,7 +7874,7 @@
         <v>1178</v>
       </c>
       <c r="D214" s="17" t="s">
-        <v>1177</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7456,7 +7885,7 @@
         <v>1180</v>
       </c>
       <c r="D215" s="17" t="s">
-        <v>1179</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>